<commit_message>
Make that standard case is shown first in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/csv/template_recovery.xlsx
+++ b/src/test/resources/csv/template_recovery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedricmoullet/sandbox/CovidCertificate-Management-Service/src/test/resources/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F602825D-0137-6248-9B12-86A8D703CB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8076028-6F3C-5644-A981-F6CAA31B1159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recovery" sheetId="2" r:id="rId1"/>
@@ -918,9 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -981,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>